<commit_message>
Add SIMPLE BASIC UI Sprite auto import settings. Sprite batch modify tool.
</commit_message>
<xml_diff>
--- a/Product/SettingSource/I18N/en_US.xlsx
+++ b/Product/SettingSource/I18N/en_US.xlsx
@@ -1,6 +1,113 @@
 
-<file path=theme/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>CommentSrcFile</t>
+  </si>
+  <si>
+    <t>string/int/pk</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>原文</t>
+  </si>
+  <si>
+    <t>翻译</t>
+  </si>
+  <si>
+    <t>出处</t>
+  </si>
+  <si>
+    <t>StartGame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>START_GAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10,39 +117,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -121,131 +228,160 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -255,6 +391,86 @@
 </a:theme>
 </file>
 
-<file path=theme/theme/themeManager.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeManager xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Recompile TableMLCompiler to extend xls cs template.Add for template for C# Array.Complete a role card.
</commit_message>
<xml_diff>
--- a/Product/SettingSource/I18N/en_US.xlsx
+++ b/Product/SettingSource/I18N/en_US.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -55,6 +55,10 @@
   </si>
   <si>
     <t>ZHAOYUN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAOCAO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,13 +405,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="44.25" customWidth="1"/>
+    <col min="2" max="2" width="76.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -456,6 +464,14 @@
       </c>
       <c r="B5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>